<commit_message>
Updated files and added new assets
</commit_message>
<xml_diff>
--- a/src/backend/contacts.xlsx
+++ b/src/backend/contacts.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -479,9 +479,77 @@
         <v>hark</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>2025-04-03T19:32:30.695Z</v>
+      </c>
+      <c r="B5" t="str">
+        <v>pravin</v>
+      </c>
+      <c r="C5" t="str">
+        <v>pravin@gmail.com</v>
+      </c>
+      <c r="D5" t="str">
+        <v>8363788798</v>
+      </c>
+      <c r="E5" t="str">
+        <v>pravin</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>2025-04-03T19:32:34.490Z</v>
+      </c>
+      <c r="B6" t="str">
+        <v>pravin</v>
+      </c>
+      <c r="C6" t="str">
+        <v>pravin@gmail.com</v>
+      </c>
+      <c r="D6" t="str">
+        <v>8363788798</v>
+      </c>
+      <c r="E6" t="str">
+        <v>pravin</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>2025-04-03T19:32:37.592Z</v>
+      </c>
+      <c r="B7" t="str">
+        <v>pravin</v>
+      </c>
+      <c r="C7" t="str">
+        <v>pravin@gmail.com</v>
+      </c>
+      <c r="D7" t="str">
+        <v>8363788798</v>
+      </c>
+      <c r="E7" t="str">
+        <v>pravin</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>2025-04-03T19:34:12.873Z</v>
+      </c>
+      <c r="B8" t="str">
+        <v>pravin</v>
+      </c>
+      <c r="C8" t="str">
+        <v>pravin@gmail.com</v>
+      </c>
+      <c r="D8" t="str">
+        <v>8363788798</v>
+      </c>
+      <c r="E8" t="str">
+        <v>fff</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>